<commit_message>
pused from hp system
</commit_message>
<xml_diff>
--- a/src/main/resources/com/aperture/test/AppertureDataProvider.xlsx
+++ b/src/main/resources/com/aperture/test/AppertureDataProvider.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vandana.jain\eclipse-workspace\gspann.aperture\src\main\resources\com\aperture\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B039E206-A3B8-4F8F-BA26-D1ACABF5EB1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BBFF92-FB92-4FD4-954B-025540C2C7E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{4C2C6DE9-97B0-4468-AD11-A0FD61BE8865}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" xr2:uid="{4C2C6DE9-97B0-4468-AD11-A0FD61BE8865}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TimeSheetHours" sheetId="1" r:id="rId1"/>
     <sheet name="Account" sheetId="2" r:id="rId2"/>
     <sheet name="Project" sheetId="3" r:id="rId3"/>
-    <sheet name="ProjectBugs" sheetId="8" r:id="rId4"/>
-    <sheet name="Resource" sheetId="4" r:id="rId5"/>
-    <sheet name="SOW" sheetId="5" r:id="rId6"/>
-    <sheet name="Allocation" sheetId="6" r:id="rId7"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
+    <sheet name="Resource" sheetId="4" r:id="rId4"/>
+    <sheet name="SOW" sheetId="5" r:id="rId5"/>
+    <sheet name="Allocation" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
   <si>
     <t>CustomerGroup</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Functional CMS,Commerce,Functional Commerce</t>
   </si>
   <si>
-    <t>United Health Group</t>
-  </si>
-  <si>
     <t>PHP Java Selenium</t>
   </si>
   <si>
@@ -217,24 +214,12 @@
     <t>RND</t>
   </si>
   <si>
-    <t>Vandana%Jain</t>
-  </si>
-  <si>
-    <t>Vandana$Jain</t>
-  </si>
-  <si>
     <t>Fix Bid</t>
   </si>
   <si>
     <t>United States</t>
   </si>
   <si>
-    <t>Functional CMS,Commerce,Manual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Work </t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -277,81 +262,6 @@
     <t>php java Automation Testing</t>
   </si>
   <si>
-    <t>RND#</t>
-  </si>
-  <si>
-    <t>APRTG123$</t>
-  </si>
-  <si>
-    <t>MKNZ()</t>
-  </si>
-  <si>
-    <t>Vandana@Jain</t>
-  </si>
-  <si>
-    <t>Vandana Malik</t>
-  </si>
-  <si>
-    <t>Itrack#$%</t>
-  </si>
-  <si>
-    <t>Mckenize 890</t>
-  </si>
-  <si>
-    <t>Apperture&amp;)@#&amp;$</t>
-  </si>
-  <si>
-    <t>Apperture87348912</t>
-  </si>
-  <si>
-    <t>Fix Bidded</t>
-  </si>
-  <si>
-    <t>Fixed</t>
-  </si>
-  <si>
-    <t>Investmemt</t>
-  </si>
-  <si>
-    <t>Indiaae</t>
-  </si>
-  <si>
-    <t>United</t>
-  </si>
-  <si>
-    <t>Asia</t>
-  </si>
-  <si>
-    <t>Fnctional CMS,Cmmerce,Funtional Commerce</t>
-  </si>
-  <si>
-    <t>Functional CMS,Functional CMS,Functional CMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hold </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
-  </si>
-  <si>
-    <t>PHP Java $*%*$@)</t>
-  </si>
-  <si>
-    <t>PHP 12345 Selenium php</t>
-  </si>
-  <si>
-    <t>PHP PHP PHP PHP PHP</t>
-  </si>
-  <si>
-    <t>32-Mar-18</t>
-  </si>
-  <si>
-    <t>29-Feb-19</t>
-  </si>
-  <si>
-    <t>05-05-0000</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -364,9 +274,6 @@
     <t>Tring to enter same technology repeatidly ,Testing for InValid Date</t>
   </si>
   <si>
-    <t>99-99-9999</t>
-  </si>
-  <si>
     <t>Tring to enter same Practice repeatidly ,Testing for InValid Date</t>
   </si>
   <si>
@@ -382,34 +289,37 @@
     <t>Testing for customer name that do not exist</t>
   </si>
   <si>
-    <t>Itrack()</t>
-  </si>
-  <si>
-    <t>Itrack_ _ _</t>
-  </si>
-  <si>
-    <t>Mckenize890+_)(*(</t>
-  </si>
-  <si>
-    <t>Apperture()</t>
-  </si>
-  <si>
-    <t>Apperture  mkl</t>
-  </si>
-  <si>
-    <t>Vandana,Jain</t>
-  </si>
-  <si>
-    <t>VandanaJain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rodan </t>
-  </si>
-  <si>
-    <t>eeee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Health </t>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>User submitting hours 0</t>
+  </si>
+  <si>
+    <t>User submitting hours 1</t>
+  </si>
+  <si>
+    <t>User submitting hours 2</t>
+  </si>
+  <si>
+    <t>User submitting hours 8</t>
+  </si>
+  <si>
+    <t>User submitting hours more than 8</t>
+  </si>
+  <si>
+    <t>User submitting hours more than 100</t>
+  </si>
+  <si>
+    <t>User submitting hours more than 24</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Submit timesheet</t>
   </si>
 </sst>
 </file>
@@ -794,12 +704,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12A1B48-4E64-42CF-B522-3ACBD2A2DF2C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>111</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -812,18 +839,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -849,9 +876,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -872,10 +899,10 @@
         <v>13</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -883,7 +910,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -898,7 +925,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -914,29 +941,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63512A86-9699-4A68-ACB7-C46C954E6C58}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="10" width="48.28515625" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="48.33203125" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="33.42578125" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="33.44140625" customWidth="1"/>
+    <col min="14" max="14" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -980,12 +1007,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1012,10 +1039,10 @@
         <v>34</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M2" s="3">
         <v>43225</v>
@@ -1024,21 +1051,21 @@
         <v>43444</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -1047,10 +1074,10 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J3" t="s">
         <v>34</v>
@@ -1059,7 +1086,7 @@
         <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M3" s="3">
         <v>43225</v>
@@ -1068,18 +1095,18 @@
         <v>43444</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>31</v>
@@ -1091,19 +1118,19 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
         <v>34</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M4" s="3">
         <v>43225</v>
@@ -1112,12 +1139,12 @@
         <v>43444</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1126,7 +1153,7 @@
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -1135,10 +1162,10 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s">
         <v>34</v>
@@ -1147,7 +1174,7 @@
         <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="3">
         <v>43225</v>
@@ -1163,348 +1190,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600099AC-0EB7-4966-95EA-CCFB3CCB0FDD}">
-  <dimension ref="A1:N7"/>
-  <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="48.7109375" customWidth="1"/>
-    <col min="11" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L2" t="s">
-        <v>100</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" t="s">
-        <v>101</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" t="s">
-        <v>102</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" t="s">
-        <v>93</v>
-      </c>
-      <c r="J5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L5" t="s">
-        <v>100</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" t="s">
-        <v>94</v>
-      </c>
-      <c r="J6" t="s">
-        <v>97</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>101</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" t="s">
-        <v>95</v>
-      </c>
-      <c r="J7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" t="s">
-        <v>102</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{796770B5-26F8-4E5E-8D68-25935AACB938}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{5E48B789-69DE-46FD-8D85-4DD19BDE29EF}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2592CF36-D7AF-4198-A898-5A200004A5F4}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1512,87 +1197,87 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>42</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
       </c>
       <c r="H1" t="s">
         <v>33</v>
       </c>
       <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
       </c>
       <c r="G2" s="2">
         <v>43544</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
         <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1601,19 +1286,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35596B20-6809-453E-A83A-31C8FA532A26}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2246900-9A53-439D-ADAE-767ACABBB83C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1621,21 +1306,21 @@
       <selection activeCell="H1" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8D2731-6D4B-43B2-86B8-B70271901570}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1643,60 +1328,60 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="62" customWidth="1"/>
-    <col min="2" max="2" width="96.7109375" customWidth="1"/>
+    <col min="2" max="2" width="96.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>